<commit_message>
Backup to GitHub - 2021.05.16
</commit_message>
<xml_diff>
--- a/01_Classification/03_Output/Liver_Patient_MLM_Evaluation_Clf.xlsx
+++ b/01_Classification/03_Output/Liver_Patient_MLM_Evaluation_Clf.xlsx
@@ -471,37 +471,37 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
       <c r="C2">
-        <v>0.6899999999999999</v>
+        <v>0.61</v>
       </c>
       <c r="D2">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F2">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="G2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H2">
-        <v>0.5600000000000001</v>
+        <v>0.39</v>
       </c>
       <c r="I2">
-        <v>0.78</v>
+        <v>0.77</v>
       </c>
       <c r="J2">
-        <v>0.65</v>
+        <v>0.52</v>
       </c>
       <c r="K2">
-        <v>0.63</v>
+        <v>0.54</v>
       </c>
       <c r="L2">
-        <v>0.7</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -509,37 +509,37 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>0.8100000000000001</v>
+        <v>0.82</v>
       </c>
       <c r="C3">
-        <v>0.62</v>
+        <v>0.64</v>
       </c>
       <c r="D3">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E3">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F3">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G3">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <v>0.5</v>
+        <v>0.43</v>
       </c>
       <c r="I3">
+        <v>0.87</v>
+      </c>
+      <c r="J3">
+        <v>0.58</v>
+      </c>
+      <c r="K3">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="L3">
         <v>0.71</v>
-      </c>
-      <c r="J3">
-        <v>0.59</v>
-      </c>
-      <c r="K3">
-        <v>0.57</v>
-      </c>
-      <c r="L3">
-        <v>0.64</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -547,34 +547,34 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>0.71</v>
+        <v>0.67</v>
       </c>
       <c r="C4">
-        <v>0.64</v>
+        <v>0.57</v>
       </c>
       <c r="D4">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E4">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F4">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="G4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="H4">
-        <v>0.52</v>
+        <v>0.38</v>
       </c>
       <c r="I4">
-        <v>0.78</v>
+        <v>0.9</v>
       </c>
       <c r="J4">
-        <v>0.62</v>
+        <v>0.53</v>
       </c>
       <c r="K4">
-        <v>0.55</v>
+        <v>0.44</v>
       </c>
       <c r="L4">
         <v>0.67</v>
@@ -585,37 +585,37 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>0.82</v>
+        <v>0.74</v>
       </c>
       <c r="C5">
-        <v>0.66</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D5">
+        <v>26</v>
+      </c>
+      <c r="E5">
+        <v>49</v>
+      </c>
+      <c r="F5">
         <v>30</v>
       </c>
-      <c r="E5">
-        <v>41</v>
-      </c>
-      <c r="F5">
-        <v>26</v>
-      </c>
       <c r="G5">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="H5">
-        <v>0.54</v>
+        <v>0.46</v>
       </c>
       <c r="I5">
-        <v>0.73</v>
+        <v>0.87</v>
       </c>
       <c r="J5">
+        <v>0.6</v>
+      </c>
+      <c r="K5">
         <v>0.62</v>
       </c>
-      <c r="K5">
-        <v>0.61</v>
-      </c>
       <c r="L5">
-        <v>0.67</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -623,37 +623,37 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>0.89</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="C6">
-        <v>0.64</v>
+        <v>0.53</v>
       </c>
       <c r="D6">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E6">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F6">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>0.44</v>
+        <v>0.31</v>
       </c>
       <c r="I6">
-        <v>0.93</v>
+        <v>1</v>
       </c>
       <c r="J6">
-        <v>0.6</v>
+        <v>0.47</v>
       </c>
       <c r="K6">
-        <v>0.28</v>
+        <v>0.15</v>
       </c>
       <c r="L6">
-        <v>0.61</v>
+        <v>0.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>